<commit_message>
Added SheetCellRange.get_subset() and corresponding unit tests
</commit_message>
<xml_diff>
--- a/openpyxlplus/test/test_cell_range.xlsx
+++ b/openpyxlplus/test/test_cell_range.xlsx
@@ -4,19 +4,20 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="12450"/>
+    <workbookView windowWidth="28800" windowHeight="12450" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="DefaultStyle" sheetId="4" r:id="rId3"/>
+    <sheet name="Clear" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="21">
   <si>
     <t>aa</t>
   </si>
@@ -76,6 +77,9 @@
   </si>
   <si>
     <t>Bold</t>
+  </si>
+  <si>
+    <t>color,bold,fill</t>
   </si>
 </sst>
 </file>
@@ -83,12 +87,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="22">
+  <fonts count="21">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -99,15 +103,91 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -120,60 +200,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -187,24 +223,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -218,32 +239,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -256,7 +253,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -265,19 +262,103 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -289,37 +370,55 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -331,121 +430,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -456,6 +459,45 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -477,8 +519,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -507,45 +549,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top style="thin">
@@ -559,154 +562,154 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="13" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="16" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="2" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1028,7 +1031,7 @@
   <sheetPr/>
   <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
@@ -1210,7 +1213,7 @@
   <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K16" sqref="K14:L16"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="1"/>
@@ -1227,4 +1230,40 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="1" outlineLevelCol="1"/>
+  <cols>
+    <col min="1" max="2" width="14" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Archived autofit_width. Created new method: autosize which can adjust both rows and columns.
</commit_message>
<xml_diff>
--- a/openpyxlplus/test/test_cell_range.xlsx
+++ b/openpyxlplus/test/test_cell_range.xlsx
@@ -87,8 +87,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
@@ -109,45 +109,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
+      <sz val="13"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -162,8 +125,23 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -171,22 +149,30 @@
     <font>
       <u/>
       <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
       <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -194,7 +180,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -203,29 +189,6 @@
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -239,8 +202,45 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -268,25 +268,145 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -298,7 +418,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -310,145 +442,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -459,6 +459,26 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -477,15 +497,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -497,30 +508,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -544,25 +531,38 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4"/>
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
+      <top/>
       <bottom style="double">
-        <color theme="4"/>
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -580,130 +580,130 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="23" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="13" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="13" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1238,7 +1238,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="O14" sqref="O14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="1" outlineLevelCol="1"/>

</xml_diff>